<commit_message>
Push final avec les dernières modifications
</commit_message>
<xml_diff>
--- a/Rapport d'optimisation.xlsx
+++ b/Rapport d'optimisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\Documents\Formation\Projets\P4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609C2FC2-46CC-47EA-8269-BAF543C6DA8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835BBE2E-4058-4769-982E-04A96E6E4264}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Catégorie</t>
   </si>
@@ -114,30 +114,26 @@
     <t>Après</t>
   </si>
   <si>
-    <t>Résultat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En ADSL :
-On passe de
-à
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le contraste des textes et conforme aux recommandations.
-</t>
-  </si>
-  <si>
     <t>Les balises &lt;title&gt; et &lt;description&gt; sont vides.</t>
   </si>
   <si>
     <t>Remplir les balises avec un titre et une description qui mettent en avant les mots-clés importants du site et qui décrivent la page.</t>
+  </si>
+  <si>
+    <t>Résultats des modifications :</t>
+  </si>
+  <si>
+    <t>Après les améliorations listées ci-dessus, le site ne présente plus aucune erreur aux validateurs HTML et CSS W3C.
+Les contrastes sont désormais conformes aux recommandations WGAC.
+Le temps de chargement de la page est considérablement diminué et est plus facile à crawler pour Google.
+Tous ces éléments améliorent son SEO et vont faire remonter le site sur Google.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,6 +153,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -172,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -268,21 +277,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -310,10 +304,25 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -324,32 +333,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -364,7 +347,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -378,24 +361,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -421,13 +391,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -442,7 +412,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -454,14 +424,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -672,7 +651,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9858375" y="923396"/>
+          <a:off x="10258425" y="923396"/>
           <a:ext cx="4315278" cy="1076854"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1927,16 +1906,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>638175</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1476472</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>857281</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>695324</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1923637</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1076325</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1965,8 +1944,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15420975" y="19526250"/>
-          <a:ext cx="695422" cy="219106"/>
+          <a:off x="10753725" y="24345899"/>
+          <a:ext cx="1209262" cy="381001"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1977,16 +1956,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>771525</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1219200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1466947</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1428779</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2390774</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>695325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3623397</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1066800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2015,8 +1994,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15411450" y="20107275"/>
-          <a:ext cx="695422" cy="209579"/>
+          <a:off x="12430124" y="24345900"/>
+          <a:ext cx="1232623" cy="371475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2127,23 +2106,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>588783</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1104901</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1838637</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1123950</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1809750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3677006</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2190803</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="72" name="Image 71">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DFFC047-4B39-499E-A3AA-633A1191241F}"/>
+        <xdr:cNvPr id="76" name="Image 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CA63B6B-5BED-43CA-BFE9-C77606DC83A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2165,8 +2144,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14697076" y="21467583"/>
-          <a:ext cx="1047750" cy="1249854"/>
+          <a:off x="6381750" y="2247900"/>
+          <a:ext cx="2553056" cy="381053"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2177,23 +2156,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1114425</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>580073</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2152650</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1819586</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1585609</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4638675</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2381390</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="74" name="Image 73">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D38B588B-6AF8-4B1B-A851-CAADEEF3EC09}"/>
+        <xdr:cNvPr id="78" name="Image 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7F3AB0A-309E-406D-8DB6-4A5546CE8CB6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2215,8 +2194,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15754350" y="21458873"/>
-          <a:ext cx="1038225" cy="1239513"/>
+          <a:off x="10115550" y="2023759"/>
+          <a:ext cx="4562475" cy="795781"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2227,23 +2206,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1123950</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1809750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3677006</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>2190803</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>638175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>600269</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1124018</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="76" name="Image 75">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CA63B6B-5BED-43CA-BFE9-C77606DC83A5}"/>
+        <xdr:cNvPr id="51" name="Image 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F7D9769-0E13-4D7E-A7DA-5BB6316DBA0E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2265,8 +2244,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6381750" y="2247900"/>
-          <a:ext cx="2553056" cy="381053"/>
+          <a:off x="400050" y="24288750"/>
+          <a:ext cx="1390844" cy="485843"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2277,23 +2256,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1585609</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>4638675</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>2381390</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>279358</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>809625</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1714850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="78" name="Image 77">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7F3AB0A-309E-406D-8DB6-4A5546CE8CB6}"/>
+        <xdr:cNvPr id="11" name="Image 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DFFC460-4403-4D10-A055-BE3FFF671BBA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2315,8 +2294,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10115550" y="2023759"/>
-          <a:ext cx="4562475" cy="795781"/>
+          <a:off x="2162175" y="23929933"/>
+          <a:ext cx="1457325" cy="1435492"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2327,23 +2306,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1790894</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>638243</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>503049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2343150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1676665</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="80" name="Image 79">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5C140EE-0F7A-4177-A460-C7613CCEFA1B}"/>
+        <xdr:cNvPr id="15" name="Image 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95708003-47F0-4F2E-9EC9-67213F94D5AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2365,8 +2344,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15220950" y="590550"/>
-          <a:ext cx="1390844" cy="485843"/>
+          <a:off x="3838575" y="24153624"/>
+          <a:ext cx="1314450" cy="1173616"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2375,175 +2354,25 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1219200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1790894</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1533569</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="82" name="Image 81">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B219B61D-8C51-478C-8B47-E76CB3C8B1DE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15220950" y="1657350"/>
-          <a:ext cx="1390844" cy="314369"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1885950</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1876639</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>2257477</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="84" name="Image 83">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{661014D7-C057-43BB-9BD8-DF2342A55976}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15163800" y="2324100"/>
-          <a:ext cx="1533739" cy="371527"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>638175</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2095777</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1000176</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="86" name="Image 85">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ED9D0FB-DCAF-4905-AEDB-0D28AD9451BB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14935200" y="1076325"/>
-          <a:ext cx="1981477" cy="362001"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1562100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1276350</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1857375</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>876300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1209675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="87" name="Flèche : bas 86">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74D60B63-D370-43B3-A268-BD4C00769152}"/>
+        <xdr:cNvPr id="17" name="Flèche : droite 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5807AB1F-C7C2-485E-8273-03BE3D22793D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2551,10 +2380,10 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15773400" y="2000250"/>
-          <a:ext cx="323850" cy="295275"/>
-        </a:xfrm>
-        <a:prstGeom prst="downArrow">
+          <a:off x="3581400" y="24526875"/>
+          <a:ext cx="381000" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -2580,6 +2409,661 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3924300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>594561</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Image 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{151047E5-2119-43F3-8530-5EB5DC80BC82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5953125" y="23707726"/>
+          <a:ext cx="3228975" cy="537410"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>600075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3762375</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>972158</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Image 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28AE8D71-9209-44C7-BD94-39D5AEFC9B23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6191250" y="24250650"/>
+          <a:ext cx="2828925" cy="372083"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1306979</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3714750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1638387</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Image 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F12F92A-0050-4B78-8B9D-A81A71A03DCD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6200775" y="24957554"/>
+          <a:ext cx="2771775" cy="331408"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2181225</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>990600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2505075</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1285875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="Flèche : bas 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D32120EA-1475-4890-9EBB-2EC8AE93DB43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7439025" y="24641175"/>
+          <a:ext cx="323850" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3295650</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>619124</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="ZoneTexte 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{989B3199-E84A-4660-909F-244B21BA0B57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11068050" y="23669624"/>
+          <a:ext cx="2266950" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" b="1"/>
+            <a:t>Poids de la page et temps de chargement</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1400" b="1"/>
+            <a:t>en ADSL</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1971675</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>714375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2352675</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1047750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="Flèche : droite 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B661B30-AC4A-4840-9685-9314B24102EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12011025" y="24364950"/>
+          <a:ext cx="381000" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1981200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1219200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2362200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1552575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="Flèche : droite 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B700C71F-8E35-4951-B6DA-1AEA30C4334C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12020550" y="24869775"/>
+          <a:ext cx="381000" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1247774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1953865</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1543049</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="69" name="Image 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD291BFC-0070-406A-8098-C426F1D7E2BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10696575" y="24898349"/>
+          <a:ext cx="1296640" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2409824</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1257299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3932823</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1552574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="73" name="Image 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39897C2A-9D8B-40BC-B426-9CAE74782481}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12449174" y="24907874"/>
+          <a:ext cx="1522999" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2143125</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1409701</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2381250</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1619251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="ZoneTexte 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73181E02-E632-46BD-9020-D95B81416D59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="25060276"/>
+          <a:ext cx="238125" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>*</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>2019300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>2543175</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="ZoneTexte 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5F68DB1-A1A4-4EE6-A37E-F9886DDC7589}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="361950" y="25669875"/>
+          <a:ext cx="10172700" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>* Le site n'étant pas en ligne, l'indicateur de score SEO n'est pas représentatif de sa performance réelle, car il lui manque des données à analyser telles que l'url par exemple.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Il ne sert ici qu'à montrer l'amélioration avant/après</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2786,10 +3270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y991"/>
+  <dimension ref="A1:X991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2799,11 +3283,10 @@
     <col min="3" max="3" width="28.5546875" customWidth="1"/>
     <col min="4" max="4" width="55.77734375" style="7" customWidth="1"/>
     <col min="5" max="5" width="55.77734375" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" customWidth="1"/>
-    <col min="7" max="25" width="10.5546875" customWidth="1"/>
+    <col min="6" max="24" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="2" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="2" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2816,12 +3299,10 @@
       <c r="D1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>27</v>
-      </c>
+      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2840,23 +3321,21 @@
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
     </row>
-    <row r="2" spans="1:25" ht="198.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="198.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="17"/>
-      <c r="F2" s="20"/>
     </row>
-    <row r="3" spans="1:25" ht="147" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="147" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -2868,9 +3347,8 @@
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="18"/>
-      <c r="F3" s="21"/>
     </row>
-    <row r="4" spans="1:25" ht="327" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="327" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -2882,9 +3360,8 @@
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="18"/>
-      <c r="F4" s="21"/>
     </row>
-    <row r="5" spans="1:25" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -2896,9 +3373,8 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="18"/>
-      <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="1:25" ht="193.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" ht="193.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2910,9 +3386,8 @@
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="18"/>
-      <c r="F6" s="21"/>
     </row>
-    <row r="7" spans="1:25" ht="139.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" ht="139.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -2924,9 +3399,8 @@
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="18"/>
-      <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="1:25" ht="153" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -2938,9 +3412,8 @@
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="18"/>
-      <c r="F8" s="21"/>
     </row>
-    <row r="9" spans="1:25" ht="184.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" ht="184.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -2952,9 +3425,8 @@
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="18"/>
-      <c r="F9" s="21"/>
     </row>
-    <row r="10" spans="1:25" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
@@ -2966,11 +3438,8 @@
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="21" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="11" spans="1:25" ht="153" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="153" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -2982,15 +3451,28 @@
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="19"/>
-      <c r="F11" s="22" t="s">
+    </row>
+    <row r="12" spans="1:24" ht="220.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
         <v>29</v>
       </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:24" ht="106.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25"/>
+    </row>
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3967,8 +4449,12 @@
     <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>